<commit_message>
fix: issue #80 update incorrect column names
Remove reference to versioning worksheet (versioning now tracked in git). Delete old .xls version of the input template file.
</commit_message>
<xml_diff>
--- a/inst/extdat/input-file-template.xlsx
+++ b/inst/extdat/input-file-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim.Foster\Documents\r-projects\rict\inst\extdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CE8EE3-8645-42E9-B0B5-6EB2CB92EEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6F8216-DF8C-49A4-B3CD-44E490DEEF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -40,8 +40,152 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Foster, Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E7C14446-8C03-43B7-9D80-C45FBE924E3C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D6A62A15-037E-4BDE-9C35-E8446E3419AE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Foster, Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F2D04F44-76D5-4A92-99D4-CE5260D6B0E8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D33BB43F-A723-4398-850B-1E98B4E8D8B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Foster, Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{2FFC52FA-F399-4321-B5E4-98BCF83D42EB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{919BABFF-AAAC-4B7E-8755-09A41E99C9C1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Foster, Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{29B83F55-772A-4847-9B00-7C2414BCCA0A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8E2C6CE8-068E-4489-BAB6-DC7D271DCBD1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>5-fig unless leading zeroes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="86">
   <si>
     <t>SITE</t>
   </si>
@@ -229,12 +373,6 @@
     <t>TST-GB-01-D</t>
   </si>
   <si>
-    <t>Easting (5-fig unless leading zeroes)</t>
-  </si>
-  <si>
-    <t>Northing (5-fig unless leading zeroes)</t>
-  </si>
-  <si>
     <t>MYR-GB-01-R</t>
   </si>
   <si>
@@ -311,7 +449,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +470,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -764,6 +908,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -820,13 +971,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -855,13 +999,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -897,6 +1034,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -904,34 +1048,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -967,14 +1083,42 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1089,13 +1233,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1124,6 +1261,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1132,13 +1283,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1323,6 +1467,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1351,13 +1502,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1372,6 +1516,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1379,34 +1551,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1435,6 +1579,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1505,13 +1656,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1569,13 +1713,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1599,6 +1736,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1606,13 +1750,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1655,6 +1792,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1662,13 +1806,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1683,6 +1820,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1718,13 +1862,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1739,6 +1876,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1746,13 +1904,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1767,20 +1918,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1788,6 +1925,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1837,27 +1995,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1928,6 +2065,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -1985,13 +2129,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2015,6 +2152,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2022,13 +2166,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2071,6 +2208,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2078,13 +2222,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2099,6 +2236,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2134,13 +2278,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2155,6 +2292,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2162,13 +2320,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2183,20 +2334,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2204,6 +2341,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2253,27 +2411,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -2282,6 +2419,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2317,8 +2461,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>51</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>36199</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2333,8 +2477,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="167641" y="132715"/>
-          <a:ext cx="6414134" cy="11295381"/>
+          <a:off x="205741" y="170815"/>
+          <a:ext cx="6499910" cy="10459085"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2577,7 +2721,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>3. Example test data and version history</a:t>
+            <a:t>3. Example test data</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2603,16 +2747,28 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Model 44 GB, Version history</a:t>
+            <a:t>Model 44 GB</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPts val="1300"/>
             </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="none" baseline="0">
+          <a:endParaRPr lang="en-GB" sz="1200" b="1" u="none" baseline="0">
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
@@ -3305,6 +3461,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -3594,7 +3754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3607,14 +3767,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3645,7 +3805,7 @@
     <col min="34" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="7" customFormat="1" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="7" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3659,10 +3819,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>19</v>
@@ -3773,14 +3933,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="cellIs" dxfId="264" priority="43" stopIfTrue="1" operator="greaterThan">
-      <formula>2027</formula>
+    <cfRule type="expression" dxfId="264" priority="73" stopIfTrue="1">
+      <formula>ISTEXT($C2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="263" priority="44" stopIfTrue="1" operator="lessThan">
       <formula>1990</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="73" stopIfTrue="1">
-      <formula>ISTEXT($C2)</formula>
+    <cfRule type="cellIs" dxfId="262" priority="43" stopIfTrue="1" operator="greaterThan">
+      <formula>2027</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
@@ -3810,37 +3970,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="cellIs" dxfId="255" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="100" stopIfTrue="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="254" priority="99" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="98" stopIfTrue="1" operator="greaterThan">
+      <formula>1345</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="252" priority="78" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="72" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="251" priority="101" stopIfTrue="1" operator="greaterThan">
+      <formula>590</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="250" priority="72" stopIfTrue="1">
       <formula>ISTEXT($G2)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="101" stopIfTrue="1" operator="greaterThan">
-      <formula>590</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="100" stopIfTrue="1" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="99" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="98" stopIfTrue="1" operator="greaterThan">
-      <formula>1345</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
-    <cfRule type="expression" dxfId="249" priority="71" stopIfTrue="1">
-      <formula>ISTEXT($H2)</formula>
+    <cfRule type="cellIs" dxfId="249" priority="83" stopIfTrue="1" operator="greaterThan">
+      <formula>150</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="248" priority="84" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="247" priority="71" stopIfTrue="1">
+      <formula>ISTEXT($H2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="37" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="83" stopIfTrue="1" operator="greaterThan">
-      <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I65536">
@@ -3849,25 +4009,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I65536">
-    <cfRule type="cellIs" dxfId="244" priority="70" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="244" priority="35" stopIfTrue="1">
+      <formula>ISTEXT($I2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="243" priority="70" stopIfTrue="1" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="35" stopIfTrue="1">
-      <formula>ISTEXT($I2)</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J65536">
-    <cfRule type="expression" dxfId="242" priority="9" stopIfTrue="1">
-      <formula>$I2&amp;$J2=""</formula>
+    <cfRule type="cellIs" dxfId="242" priority="30" stopIfTrue="1" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="241" priority="60" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="30" stopIfTrue="1" operator="greaterThan">
-      <formula>10</formula>
+    <cfRule type="expression" dxfId="240" priority="9" stopIfTrue="1">
+      <formula>$I2&amp;$J2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J65536">
@@ -3882,11 +4042,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65536">
-    <cfRule type="cellIs" dxfId="236" priority="94" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="236" priority="67" stopIfTrue="1">
+      <formula>ISTEXT($K2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="94" stopIfTrue="1" operator="greaterThan">
       <formula>202.8</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="235" priority="67" stopIfTrue="1">
-      <formula>ISTEXT($K2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="234" priority="95" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
@@ -3901,25 +4061,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L65536">
-    <cfRule type="cellIs" dxfId="231" priority="89" stopIfTrue="1" operator="lessThan">
-      <formula>0.4</formula>
+    <cfRule type="expression" dxfId="231" priority="66" stopIfTrue="1">
+      <formula>ISTEXT($L2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="230" priority="88" stopIfTrue="1" operator="greaterThan">
       <formula>117</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="66" stopIfTrue="1">
-      <formula>ISTEXT($L2)</formula>
+    <cfRule type="cellIs" dxfId="229" priority="89" stopIfTrue="1" operator="lessThan">
+      <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M65536">
-    <cfRule type="cellIs" dxfId="228" priority="92" stopIfTrue="1" operator="lessThan">
+    <cfRule type="expression" dxfId="228" priority="65" stopIfTrue="1">
+      <formula>ISTEXT($M2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="91" stopIfTrue="1" operator="greaterThan">
+      <formula>300</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="92" stopIfTrue="1" operator="lessThan">
       <formula>1.7</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="227" priority="65" stopIfTrue="1">
-      <formula>ISTEXT($M2)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="91" stopIfTrue="1" operator="greaterThan">
-      <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65536 S2:U65536">
@@ -3928,14 +4088,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65536">
-    <cfRule type="cellIs" dxfId="224" priority="103" stopIfTrue="1" operator="lessThan">
+    <cfRule type="expression" dxfId="224" priority="64" stopIfTrue="1">
+      <formula>ISTEXT($N2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="223" priority="103" stopIfTrue="1" operator="lessThan">
       <formula>1.2</formula>
     </cfRule>
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="223" priority="64" stopIfTrue="1">
-      <formula>ISTEXT($N2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="222" priority="102" stopIfTrue="1" operator="greaterThan">
       <formula>366</formula>
@@ -3948,28 +4108,28 @@
     <cfRule type="expression" dxfId="220" priority="59" stopIfTrue="1">
       <formula>SUM($O2:$R2)&gt;103</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="219" priority="58" stopIfTrue="1">
+      <formula>SUM($O2:$R2)&lt;97</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="97" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="77" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="58" stopIfTrue="1">
-      <formula>SUM($O2:$R2)&lt;97</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="96" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="216" priority="96" stopIfTrue="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="97" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:U65536">
+    <cfRule type="cellIs" dxfId="215" priority="62" stopIfTrue="1" operator="lessThan">
+      <formula>1.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="16" stopIfTrue="1" operator="greaterThan">
+      <formula>366</formula>
+    </cfRule>
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="16" stopIfTrue="1" operator="greaterThan">
-      <formula>366</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="62" stopIfTrue="1" operator="lessThan">
-      <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:AG65536">
@@ -4009,15 +4169,16 @@
   </conditionalFormatting>
   <pageMargins left="0.47244094488188981" right="0.43307086614173229" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,10 +4222,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>19</v>
@@ -4169,14 +4330,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="cellIs" dxfId="205" priority="26" stopIfTrue="1" operator="greaterThan">
-      <formula>2027</formula>
+    <cfRule type="expression" dxfId="205" priority="46" stopIfTrue="1">
+      <formula>ISTEXT($C2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="204" priority="27" stopIfTrue="1" operator="lessThan">
       <formula>1990</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="46" stopIfTrue="1">
-      <formula>ISTEXT($C2)</formula>
+    <cfRule type="cellIs" dxfId="203" priority="26" stopIfTrue="1" operator="greaterThan">
+      <formula>2027</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
@@ -4206,37 +4367,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="cellIs" dxfId="196" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="69" stopIfTrue="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="68" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="67" stopIfTrue="1" operator="greaterThan">
+      <formula>850</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="51" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="45" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="192" priority="70" stopIfTrue="1" operator="greaterThan">
+      <formula>180</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="45" stopIfTrue="1">
       <formula>ISTEXT($G2)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="70" stopIfTrue="1" operator="greaterThan">
-      <formula>180</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="69" stopIfTrue="1" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="68" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="67" stopIfTrue="1" operator="greaterThan">
-      <formula>850</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
-    <cfRule type="expression" dxfId="190" priority="44" stopIfTrue="1">
-      <formula>ISTEXT($H2)</formula>
+    <cfRule type="cellIs" dxfId="190" priority="54" stopIfTrue="1" operator="greaterThan">
+      <formula>50</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="189" priority="55" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="188" priority="44" stopIfTrue="1">
+      <formula>ISTEXT($H2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="22" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="54" stopIfTrue="1" operator="greaterThan">
-      <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I65536">
@@ -4245,25 +4406,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I65536">
-    <cfRule type="cellIs" dxfId="185" priority="43" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="185" priority="20" stopIfTrue="1">
+      <formula>ISTEXT($I2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="184" priority="43" stopIfTrue="1" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="20" stopIfTrue="1">
-      <formula>ISTEXT($I2)</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J65536">
-    <cfRule type="expression" dxfId="183" priority="5" stopIfTrue="1">
-      <formula>$I2&amp;$J2=""</formula>
+    <cfRule type="cellIs" dxfId="183" priority="15" stopIfTrue="1" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="182" priority="33" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="15" stopIfTrue="1" operator="greaterThan">
-      <formula>10</formula>
+    <cfRule type="expression" dxfId="181" priority="5" stopIfTrue="1">
+      <formula>$I2&amp;$J2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J65536">
@@ -4278,11 +4439,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65536">
-    <cfRule type="cellIs" dxfId="177" priority="63" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="177" priority="40" stopIfTrue="1">
+      <formula>ISTEXT($K2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="63" stopIfTrue="1" operator="greaterThan">
       <formula>75</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="176" priority="40" stopIfTrue="1">
-      <formula>ISTEXT($K2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="175" priority="64" stopIfTrue="1" operator="lessThan">
       <formula>2.2</formula>
@@ -4297,25 +4458,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L65536">
-    <cfRule type="cellIs" dxfId="172" priority="58" stopIfTrue="1" operator="lessThan">
-      <formula>2</formula>
+    <cfRule type="expression" dxfId="172" priority="39" stopIfTrue="1">
+      <formula>ISTEXT($L2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="171" priority="57" stopIfTrue="1" operator="greaterThan">
       <formula>37.2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="39" stopIfTrue="1">
-      <formula>ISTEXT($L2)</formula>
+    <cfRule type="cellIs" dxfId="170" priority="58" stopIfTrue="1" operator="lessThan">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M65536">
-    <cfRule type="cellIs" dxfId="169" priority="61" stopIfTrue="1" operator="lessThan">
+    <cfRule type="expression" dxfId="169" priority="38" stopIfTrue="1">
+      <formula>ISTEXT($M2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="60" stopIfTrue="1" operator="greaterThan">
+      <formula>183</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="61" stopIfTrue="1" operator="lessThan">
       <formula>15</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="168" priority="38" stopIfTrue="1">
-      <formula>ISTEXT($M2)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="60" stopIfTrue="1" operator="greaterThan">
-      <formula>183</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65536 S2:U65536">
@@ -4324,14 +4485,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65536">
-    <cfRule type="cellIs" dxfId="165" priority="72" stopIfTrue="1" operator="lessThan">
+    <cfRule type="expression" dxfId="165" priority="37" stopIfTrue="1">
+      <formula>ISTEXT($N2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="72" stopIfTrue="1" operator="lessThan">
       <formula>0.7</formula>
     </cfRule>
     <cfRule type="cellIs" priority="12" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="164" priority="37" stopIfTrue="1">
-      <formula>ISTEXT($N2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="163" priority="71" stopIfTrue="1" operator="greaterThan">
       <formula>130</formula>
@@ -4344,28 +4505,28 @@
     <cfRule type="expression" dxfId="161" priority="32" stopIfTrue="1">
       <formula>SUM($O2:$R2)&gt;103</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="160" priority="31" stopIfTrue="1">
+      <formula>SUM($O2:$R2)&lt;97</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="66" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="50" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="31" stopIfTrue="1">
-      <formula>SUM($O2:$R2)&lt;97</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="65" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="65" stopIfTrue="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="66" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:U65536">
+    <cfRule type="cellIs" dxfId="156" priority="35" stopIfTrue="1" operator="lessThan">
+      <formula>1.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="11" stopIfTrue="1" operator="greaterThan">
+      <formula>366</formula>
+    </cfRule>
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="11" stopIfTrue="1" operator="greaterThan">
-      <formula>366</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="35" stopIfTrue="1" operator="lessThan">
-      <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:AG65536">
@@ -4404,15 +4565,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4454,10 +4616,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>19</v>
@@ -4541,14 +4703,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="expression" dxfId="146" priority="42" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="146" priority="22" stopIfTrue="1" operator="greaterThan">
+      <formula>2027</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="23" stopIfTrue="1" operator="lessThan">
+      <formula>1990</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="42" stopIfTrue="1">
       <formula>ISTEXT($C2)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="22" stopIfTrue="1" operator="greaterThan">
-      <formula>2027</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="23" stopIfTrue="1" operator="lessThan">
-      <formula>1990</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D65536">
@@ -4563,23 +4725,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="cellIs" dxfId="140" priority="65" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="66" stopIfTrue="1" operator="greaterThan">
+      <formula>113</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="65" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="64" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="64" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="63" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="63" stopIfTrue="1" operator="greaterThan">
       <formula>621</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="47" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
     </cfRule>
     <cfRule type="expression" dxfId="136" priority="41" stopIfTrue="1">
       <formula>ISTEXT($G2)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="66" stopIfTrue="1" operator="greaterThan">
-      <formula>113</formula>
+    <cfRule type="cellIs" dxfId="135" priority="47" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
@@ -4602,36 +4764,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I65536">
-    <cfRule type="expression" dxfId="129" priority="16" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="129" priority="39" stopIfTrue="1" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="16" stopIfTrue="1">
       <formula>ISTEXT($I2)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="39" stopIfTrue="1" operator="greaterThan">
-      <formula>9</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J65536">
-    <cfRule type="expression" dxfId="127" priority="1" stopIfTrue="1">
-      <formula>$I2&amp;$J2=""</formula>
+    <cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="11" stopIfTrue="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="126" priority="29" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="11" stopIfTrue="1" operator="greaterThan">
-      <formula>10</formula>
+    <cfRule type="expression" dxfId="125" priority="1" stopIfTrue="1">
+      <formula>$I2&amp;$J2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J65536">
-    <cfRule type="expression" dxfId="124" priority="49" stopIfTrue="1">
-      <formula>ISTEXT($J2)</formula>
+    <cfRule type="cellIs" dxfId="124" priority="38" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="123" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="38" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
+    <cfRule type="expression" dxfId="122" priority="49" stopIfTrue="1">
+      <formula>ISTEXT($J2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65536">
@@ -4663,19 +4825,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:O65536">
+    <cfRule type="cellIs" dxfId="113" priority="30" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="30" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O65536">
-    <cfRule type="cellIs" dxfId="112" priority="31" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="7" stopIfTrue="1" operator="greaterThan">
+      <formula>366</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="31" stopIfTrue="1" operator="lessThan">
       <formula>1.2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="7" stopIfTrue="1" operator="greaterThan">
-      <formula>366</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:AA65536 E2:F65536">
@@ -4715,15 +4877,16 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4897,33 +5060,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="expression" dxfId="102" priority="39" stopIfTrue="1">
-      <formula>ISTEXT($C2)</formula>
+    <cfRule type="cellIs" dxfId="102" priority="37" stopIfTrue="1" operator="greaterThan">
+      <formula>2027</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="101" priority="38" stopIfTrue="1" operator="lessThan">
       <formula>1990</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="37" stopIfTrue="1" operator="greaterThan">
-      <formula>2027</formula>
+    <cfRule type="expression" dxfId="100" priority="39" stopIfTrue="1">
+      <formula>ISTEXT($C2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="cellIs" dxfId="99" priority="36" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
+    <cfRule type="expression" dxfId="99" priority="34" stopIfTrue="1">
+      <formula>ISNUMBER($D2)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="98" priority="35" stopIfTrue="1">
       <formula>LEN($D2)&lt;&gt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="34" stopIfTrue="1">
-      <formula>ISNUMBER($D2)</formula>
+    <cfRule type="cellIs" dxfId="97" priority="36" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="cellIs" dxfId="96" priority="32" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="96" priority="31" stopIfTrue="1">
+      <formula>ISTEXT($N2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="32" stopIfTrue="1" operator="greaterThan">
       <formula>366</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="31" stopIfTrue="1">
-      <formula>ISTEXT($N2)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="94" priority="33" stopIfTrue="1" operator="lessThan">
       <formula>1.2</formula>
@@ -4990,6 +5153,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5135,7 +5299,7 @@
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2"/>
       <c r="C2">
@@ -5226,7 +5390,7 @@
     </row>
     <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3"/>
       <c r="C3">
@@ -5317,7 +5481,7 @@
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4"/>
       <c r="C4">
@@ -5408,7 +5572,7 @@
     </row>
     <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5"/>
       <c r="C5">
@@ -5499,7 +5663,7 @@
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6"/>
       <c r="C6">
@@ -5590,7 +5754,7 @@
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7"/>
       <c r="C7">
@@ -5681,7 +5845,7 @@
     </row>
     <row r="8" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8"/>
       <c r="C8">
@@ -5772,7 +5936,7 @@
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9"/>
       <c r="C9">
@@ -5863,7 +6027,7 @@
     </row>
     <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10"/>
       <c r="C10">
@@ -5954,7 +6118,7 @@
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11"/>
       <c r="C11">
@@ -6045,7 +6209,7 @@
     </row>
     <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12"/>
       <c r="C12">
@@ -6136,7 +6300,7 @@
     </row>
     <row r="13" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13"/>
       <c r="C13">
@@ -6227,7 +6391,7 @@
     </row>
     <row r="14" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14"/>
       <c r="C14">
@@ -6318,7 +6482,7 @@
     </row>
     <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15"/>
       <c r="C15">
@@ -6409,7 +6573,7 @@
     </row>
     <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16"/>
       <c r="C16">
@@ -6500,7 +6664,7 @@
     </row>
     <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17"/>
       <c r="C17">
@@ -6591,7 +6755,7 @@
     </row>
     <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18"/>
       <c r="C18">
@@ -6682,7 +6846,7 @@
     </row>
     <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19"/>
       <c r="C19">
@@ -6773,7 +6937,7 @@
     </row>
     <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20"/>
       <c r="C20">
@@ -6864,7 +7028,7 @@
     </row>
     <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21"/>
       <c r="C21">
@@ -6955,7 +7119,7 @@
     </row>
     <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22"/>
       <c r="C22">
@@ -7046,7 +7210,7 @@
     </row>
     <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23"/>
       <c r="C23">
@@ -7137,7 +7301,7 @@
     </row>
     <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24"/>
       <c r="C24">
@@ -7228,7 +7392,7 @@
     </row>
     <row r="25" spans="1:33" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B25"/>
       <c r="C25">
@@ -7327,53 +7491,53 @@
     <cfRule type="cellIs" dxfId="80" priority="22" stopIfTrue="1" operator="greaterThan">
       <formula>2027</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="42" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="79" priority="23" stopIfTrue="1" operator="lessThan">
+      <formula>1990</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
       <formula>ISTEXT($C2)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="23" stopIfTrue="1" operator="lessThan">
-      <formula>1990</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="cellIs" dxfId="77" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="77" priority="19" stopIfTrue="1">
+      <formula>ISNUMBER($D2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="20" stopIfTrue="1">
+      <formula>LEN($D2)&lt;&gt;2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="21" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="19" stopIfTrue="1">
-      <formula>ISNUMBER($D2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="20" stopIfTrue="1">
-      <formula>LEN($D2)&lt;&gt;2</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="cellIs" dxfId="74" priority="66" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="64" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="63" stopIfTrue="1" operator="greaterThan">
+      <formula>1345</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="47" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="41" stopIfTrue="1">
+      <formula>ISTEXT($G2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="65" stopIfTrue="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="66" stopIfTrue="1" operator="greaterThan">
       <formula>590</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="65" stopIfTrue="1" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="64" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="63" stopIfTrue="1" operator="greaterThan">
-      <formula>1345</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="47" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="41" stopIfTrue="1">
-      <formula>ISTEXT($G2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
     <cfRule type="cellIs" dxfId="68" priority="51" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="50" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="18" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="50" stopIfTrue="1" operator="greaterThan">
       <formula>150</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="18" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
     </cfRule>
     <cfRule type="expression" dxfId="65" priority="40" stopIfTrue="1">
       <formula>ISTEXT($H2)</formula>
@@ -7385,11 +7549,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I65536">
-    <cfRule type="cellIs" dxfId="63" priority="39" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="expression" dxfId="63" priority="16" stopIfTrue="1">
+      <formula>ISTEXT($I2)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="39" stopIfTrue="1" operator="greaterThan">
       <formula>9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="16" stopIfTrue="1">
-      <formula>ISTEXT($I2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J65536">
@@ -7418,30 +7582,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65536">
-    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
-      <formula>ISTEXT($K2)</formula>
+    <cfRule type="cellIs" dxfId="55" priority="60" stopIfTrue="1" operator="lessThan">
+      <formula>0.1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="54" priority="59" stopIfTrue="1" operator="greaterThan">
       <formula>202.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="60" stopIfTrue="1" operator="lessThan">
-      <formula>0.1</formula>
+    <cfRule type="expression" dxfId="53" priority="36" stopIfTrue="1">
+      <formula>ISTEXT($K2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:M65536">
-    <cfRule type="cellIs" dxfId="52" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="43" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L65536">
-    <cfRule type="expression" dxfId="50" priority="35" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="50" priority="54" stopIfTrue="1" operator="lessThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="35" stopIfTrue="1">
       <formula>ISTEXT($L2)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="54" stopIfTrue="1" operator="lessThan">
-      <formula>0.4</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="48" priority="53" stopIfTrue="1" operator="greaterThan">
       <formula>117</formula>
@@ -7464,11 +7628,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65536">
+    <cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="43" priority="33" stopIfTrue="1">
       <formula>ISTEXT($N2)</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="42" priority="67" stopIfTrue="1" operator="greaterThan">
       <formula>366</formula>
@@ -7486,14 +7650,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R65536">
-    <cfRule type="cellIs" dxfId="38" priority="62" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
+    <cfRule type="cellIs" dxfId="38" priority="46" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="37" priority="61" stopIfTrue="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="46" stopIfTrue="1" operator="equal">
-      <formula>""</formula>
+    <cfRule type="cellIs" dxfId="36" priority="62" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="35" priority="32" stopIfTrue="1">
       <formula>ISTEXT(O2)</formula>
@@ -7508,14 +7672,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:U65536">
+    <cfRule type="cellIs" dxfId="32" priority="7" stopIfTrue="1" operator="greaterThan">
+      <formula>366</formula>
+    </cfRule>
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="31" stopIfTrue="1" operator="lessThan">
       <formula>1.2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="7" stopIfTrue="1" operator="greaterThan">
-      <formula>366</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:AG65536 E2:F65536">
@@ -8468,7 +8632,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11">
         <v>2018</v>
@@ -8554,7 +8718,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12">
         <v>2016</v>
@@ -8640,7 +8804,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13">
         <v>2018</v>
@@ -9500,7 +9664,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>2018</v>
@@ -9586,7 +9750,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24">
         <v>2016</v>
@@ -9672,7 +9836,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>2018</v>
@@ -9890,16 +10054,16 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2">
         <v>40000</v>
@@ -9961,16 +10125,16 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3">
         <v>2017</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3">
         <v>40000</v>
@@ -10032,16 +10196,16 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>40000</v>
@@ -10103,16 +10267,16 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>2016</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5">
         <v>39840</v>
@@ -10174,16 +10338,16 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>39840</v>
@@ -10245,16 +10409,16 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7">
         <v>39840</v>
@@ -10316,16 +10480,16 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8">
         <v>25800</v>
@@ -10387,16 +10551,16 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E9">
         <v>39000</v>
@@ -10458,16 +10622,16 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E10">
         <v>39000</v>
@@ -10529,16 +10693,16 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>2018</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11">
         <v>39000</v>
@@ -10600,16 +10764,16 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E12">
         <v>35840</v>
@@ -10671,16 +10835,16 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13">
         <v>2018</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E13">
         <v>35840</v>
@@ -10742,16 +10906,16 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>2016</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14">
         <v>40000</v>
@@ -10813,16 +10977,16 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>2017</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>40000</v>
@@ -10884,16 +11048,16 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16">
         <v>2018</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E16">
         <v>40000</v>
@@ -10955,16 +11119,16 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17">
         <v>2016</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E17">
         <v>39840</v>
@@ -11026,16 +11190,16 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>2017</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E18">
         <v>39840</v>
@@ -11097,16 +11261,16 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19">
         <v>2018</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19">
         <v>39840</v>
@@ -11168,16 +11332,16 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20">
         <v>2017</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E20">
         <v>25800</v>
@@ -11239,16 +11403,16 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21">
         <v>2016</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <v>39000</v>
@@ -11310,16 +11474,16 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22">
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22">
         <v>39000</v>
@@ -11381,16 +11545,16 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23">
         <v>2018</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>39000</v>
@@ -11452,16 +11616,16 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24">
         <v>2016</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24">
         <v>35840</v>
@@ -11523,16 +11687,16 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25">
         <v>2018</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E25">
         <v>35840</v>
@@ -11603,7 +11767,7 @@
   <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>